<commit_message>
fix: Member table sync, My Account display, QR dep
</commit_message>
<xml_diff>
--- a/data/transactions.xlsx
+++ b/data/transactions.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="144">
   <si>
     <t>transaction_id</t>
   </si>
@@ -131,6 +131,9 @@
   </si>
   <si>
     <t>TX-20260117192957</t>
+  </si>
+  <si>
+    <t>TX-20260117201635</t>
   </si>
   <si>
     <t>GDL-006</t>
@@ -800,7 +803,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -843,22 +846,22 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -866,22 +869,25 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E3" t="s">
-        <v>119</v>
+        <v>120</v>
+      </c>
+      <c r="G3">
+        <v>1234567899</v>
       </c>
       <c r="H3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -889,22 +895,22 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H4" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J4" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -912,22 +918,22 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H5" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J5" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -935,22 +941,22 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C6" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D6" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E6" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="H6" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J6" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -958,22 +964,22 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C7" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D7" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E7" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="H7" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J7" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -981,22 +987,22 @@
         <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C8" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D8" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E8" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H8" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J8" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1004,22 +1010,25 @@
         <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E9" t="s">
-        <v>119</v>
+        <v>120</v>
+      </c>
+      <c r="G9">
+        <v>1234567899</v>
       </c>
       <c r="H9" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J9" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -1027,22 +1036,22 @@
         <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C10" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D10" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E10" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H10" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J10" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1050,22 +1059,22 @@
         <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C11" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D11" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E11" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H11" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J11" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -1073,22 +1082,22 @@
         <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C12" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D12" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E12" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H12" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J12" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -1096,22 +1105,22 @@
         <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C13" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D13" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E13" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H13" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J13" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -1119,22 +1128,22 @@
         <v>22</v>
       </c>
       <c r="B14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C14" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D14" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E14" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H14" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J14" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -1142,22 +1151,22 @@
         <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C15" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E15" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H15" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J15" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -1165,22 +1174,22 @@
         <v>24</v>
       </c>
       <c r="B16" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C16" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D16" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E16" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H16" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J16" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -1188,22 +1197,22 @@
         <v>25</v>
       </c>
       <c r="B17" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C17" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D17" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E17" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H17" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J17" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -1211,22 +1220,22 @@
         <v>26</v>
       </c>
       <c r="B18" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C18" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D18" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E18" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H18" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J18" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -1234,22 +1243,22 @@
         <v>27</v>
       </c>
       <c r="B19" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C19" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D19" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E19" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H19" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J19" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1257,22 +1266,22 @@
         <v>28</v>
       </c>
       <c r="B20" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C20" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D20" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E20" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H20" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J20" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1280,22 +1289,22 @@
         <v>29</v>
       </c>
       <c r="B21" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C21" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D21" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E21" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H21" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J21" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1303,22 +1312,22 @@
         <v>30</v>
       </c>
       <c r="B22" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C22" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D22" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E22" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H22" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J22" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1326,22 +1335,22 @@
         <v>31</v>
       </c>
       <c r="B23" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C23" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D23" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E23" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H23" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J23" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -1349,22 +1358,22 @@
         <v>32</v>
       </c>
       <c r="B24" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C24" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D24" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E24" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H24" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J24" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -1372,22 +1381,22 @@
         <v>33</v>
       </c>
       <c r="B25" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C25" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D25" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E25" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H25" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J25" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -1395,22 +1404,22 @@
         <v>34</v>
       </c>
       <c r="B26" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C26" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D26" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E26" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H26" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J26" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -1418,22 +1427,22 @@
         <v>35</v>
       </c>
       <c r="B27" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C27" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D27" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E27" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H27" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J27" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -1441,22 +1450,22 @@
         <v>36</v>
       </c>
       <c r="B28" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C28" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D28" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E28" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="H28" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J28" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -1464,31 +1473,31 @@
         <v>37</v>
       </c>
       <c r="B29" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C29" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D29" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E29" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F29" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="G29">
         <v>9080314434</v>
       </c>
       <c r="H29" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="I29" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J29" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -1496,31 +1505,60 @@
         <v>38</v>
       </c>
       <c r="B30" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C30" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D30" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E30" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F30" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="G30">
         <v>9080314434</v>
       </c>
       <c r="H30" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="I30" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J30" t="s">
-        <v>142</v>
+        <v>143</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" t="s">
+        <v>68</v>
+      </c>
+      <c r="C31" t="s">
+        <v>97</v>
+      </c>
+      <c r="D31" t="s">
+        <v>99</v>
+      </c>
+      <c r="E31" t="s">
+        <v>120</v>
+      </c>
+      <c r="G31">
+        <v>1234567899</v>
+      </c>
+      <c r="H31" t="s">
+        <v>141</v>
+      </c>
+      <c r="I31" t="s">
+        <v>141</v>
+      </c>
+      <c r="J31" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>